<commit_message>
add area to Q files stn 02
</commit_message>
<xml_diff>
--- a/Discharge/Station2_2022-06-30_1235.xlsx
+++ b/Discharge/Station2_2022-06-30_1235.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Discharge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cba20500feb7d90/Documents/LongTermData_CayambeCoca/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB79E20-7ED0-724E-98D5-CB35DCA6AB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{BCB79E20-7ED0-724E-98D5-CB35DCA6AB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{743F468A-F3B5-4E43-9CEF-DBFEF45A8855}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15680" xr2:uid="{F9F41897-CA34-1E4C-9BA8-8C30B762888A}"/>
+    <workbookView xWindow="5560" yWindow="430" windowWidth="14640" windowHeight="9730" xr2:uid="{F9F41897-CA34-1E4C-9BA8-8C30B762888A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
@@ -53,6 +52,12 @@
   </si>
   <si>
     <t>Qtotal</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Atotal</t>
   </si>
 </sst>
 </file>
@@ -404,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D3C908-76FD-334C-8544-5DE1E64AA244}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +436,20 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>25</v>
       </c>
@@ -450,8 +467,24 @@
         <f>SUM(E2:E20)</f>
         <v>1.213E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <f>(D2-0)*B2/100</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(G2:G11)</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J2">
+        <f>H2</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K2">
+        <f>F2</f>
+        <v>1.213E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>30</v>
       </c>
@@ -469,8 +502,12 @@
         <f t="shared" ref="E3:E19" si="0">(D3-D2)*(B3/100)*C3</f>
         <v>1.949999999999999E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f>(D3-D2)*B3/100</f>
+        <v>2.9999999999999983E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>35</v>
       </c>
@@ -488,8 +525,12 @@
         <f t="shared" si="0"/>
         <v>3.300000000000003E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f t="shared" ref="G4:G15" si="1">(D4-D3)*B4/100</f>
+        <v>6.0000000000000053E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>40</v>
       </c>
@@ -507,8 +548,12 @@
         <f>(D5-D4)*(B5/100)*C5</f>
         <v>2.8000000000000026E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>45</v>
       </c>
@@ -519,15 +564,19 @@
         <v>0.09</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D19" si="1">(A6/100+(A7/100-A6/100)/2)</f>
+        <f t="shared" ref="D6:D19" si="2">(A6/100+(A7/100-A6/100)/2)</f>
         <v>0.47499999999999998</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
         <v>1.0799999999999985E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999985E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>50</v>
       </c>
@@ -538,15 +587,19 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52500000000000002</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
         <v>8.4000000000000079E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>55</v>
       </c>
@@ -557,15 +610,19 @@
         <v>0.36</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.57499999999999996</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>2.159999999999997E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999923E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>60</v>
       </c>
@@ -576,77 +633,105 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
@@ -654,9 +739,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E17">
@@ -664,9 +749,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18">
@@ -674,9 +759,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E19">

</xml_diff>